<commit_message>
fixed erd, table design, sql script
</commit_message>
<xml_diff>
--- a/php/tam-v.anh/doc/detail_design/db/MiniBlog_Database_Design.xlsx
+++ b/php/tam-v.anh/doc/detail_design/db/MiniBlog_Database_Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -14,96 +14,97 @@
     <sheet name="edition" sheetId="36" state="hidden" r:id="rId5"/>
     <sheet name="x_edition_version" sheetId="37" state="hidden" r:id="rId6"/>
     <sheet name="ranking(deleted)" sheetId="20" state="hidden" r:id="rId7"/>
-    <sheet name="blog" sheetId="65" r:id="rId8"/>
+    <sheet name="post" sheetId="65" r:id="rId8"/>
     <sheet name="comment" sheetId="66" r:id="rId9"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
-    <definedName name="⑫画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="4">#REF!</definedName>
+    <definedName name="⑫画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑫画面" localSheetId="5">#REF!</definedName>
-    <definedName name="②画面" localSheetId="7">#REF!</definedName>
     <definedName name="②画面" localSheetId="8">#REF!</definedName>
     <definedName name="②画面" localSheetId="4">#REF!</definedName>
+    <definedName name="②画面" localSheetId="7">#REF!</definedName>
     <definedName name="②画面" localSheetId="6">#REF!</definedName>
     <definedName name="②画面" localSheetId="5">#REF!</definedName>
-    <definedName name="③画面" localSheetId="7">#REF!</definedName>
     <definedName name="③画面" localSheetId="8">#REF!</definedName>
     <definedName name="③画面" localSheetId="4">#REF!</definedName>
+    <definedName name="③画面" localSheetId="7">#REF!</definedName>
     <definedName name="③画面" localSheetId="6">#REF!</definedName>
     <definedName name="③画面" localSheetId="5">#REF!</definedName>
-    <definedName name="⑤画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="4">#REF!</definedName>
+    <definedName name="⑤画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑤画面" localSheetId="5">#REF!</definedName>
-    <definedName name="⑧画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="4">#REF!</definedName>
+    <definedName name="⑧画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑧画面" localSheetId="5">#REF!</definedName>
-    <definedName name="⑨画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="8">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="4">#REF!</definedName>
+    <definedName name="⑨画面" localSheetId="7">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="6">#REF!</definedName>
     <definedName name="⑨画面" localSheetId="5">#REF!</definedName>
-    <definedName name="AAAAAA" localSheetId="7">#REF!</definedName>
     <definedName name="AAAAAA" localSheetId="8">#REF!</definedName>
     <definedName name="AAAAAA" localSheetId="4">#REF!</definedName>
+    <definedName name="AAAAAA" localSheetId="7">#REF!</definedName>
     <definedName name="AAAAAA" localSheetId="5">#REF!</definedName>
     <definedName name="AAAAAA">#REF!</definedName>
-    <definedName name="as" localSheetId="7">#REF!</definedName>
     <definedName name="as" localSheetId="8">#REF!</definedName>
     <definedName name="as" localSheetId="4">#REF!</definedName>
+    <definedName name="as" localSheetId="7">#REF!</definedName>
     <definedName name="as" localSheetId="5">#REF!</definedName>
     <definedName name="as">#REF!</definedName>
-    <definedName name="blog">blog!$A$1</definedName>
+    <definedName name="blog">post!$A$1</definedName>
     <definedName name="comment">comment!$A$1</definedName>
-    <definedName name="ｄｄｄｄ" localSheetId="7">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="8">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="4">#REF!</definedName>
+    <definedName name="ｄｄｄｄ" localSheetId="7">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="6">#REF!</definedName>
     <definedName name="ｄｄｄｄ" localSheetId="5">#REF!</definedName>
     <definedName name="ｄｄｄｄ">#REF!</definedName>
-    <definedName name="ｄｄｄｄｄ" localSheetId="7">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="8">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="4">#REF!</definedName>
+    <definedName name="ｄｄｄｄｄ" localSheetId="7">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="6">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ" localSheetId="5">#REF!</definedName>
     <definedName name="ｄｄｄｄｄ">#REF!</definedName>
     <definedName name="MySQL_DataType">[1]データタイプ!$B$2:$B$36</definedName>
     <definedName name="Oracle_DataType">[1]データタイプ!$A$2:$A$24</definedName>
-    <definedName name="あ" localSheetId="7">#REF!</definedName>
+    <definedName name="post">post!$A$1</definedName>
     <definedName name="あ" localSheetId="8">#REF!</definedName>
     <definedName name="あ" localSheetId="4">#REF!</definedName>
+    <definedName name="あ" localSheetId="7">#REF!</definedName>
     <definedName name="あ" localSheetId="6">#REF!</definedName>
     <definedName name="あ" localSheetId="5">#REF!</definedName>
     <definedName name="あ">#REF!</definedName>
-    <definedName name="ステータス" localSheetId="7">#REF!</definedName>
     <definedName name="ステータス" localSheetId="8">#REF!</definedName>
     <definedName name="ステータス" localSheetId="4">#REF!</definedName>
+    <definedName name="ステータス" localSheetId="7">#REF!</definedName>
     <definedName name="ステータス" localSheetId="6">#REF!</definedName>
     <definedName name="ステータス" localSheetId="5">#REF!</definedName>
     <definedName name="ステータス">#REF!</definedName>
-    <definedName name="画面一覧" localSheetId="7">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="8">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="4">#REF!</definedName>
+    <definedName name="画面一覧" localSheetId="7">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="6">#REF!</definedName>
     <definedName name="画面一覧" localSheetId="5">#REF!</definedName>
     <definedName name="画面一覧">#REF!</definedName>
-    <definedName name="項番17" localSheetId="7">#REF!</definedName>
     <definedName name="項番17" localSheetId="8">#REF!</definedName>
     <definedName name="項番17" localSheetId="4">#REF!</definedName>
+    <definedName name="項番17" localSheetId="7">#REF!</definedName>
     <definedName name="項番17" localSheetId="6">#REF!</definedName>
     <definedName name="項番17" localSheetId="5">#REF!</definedName>
     <definedName name="項番17">#REF!</definedName>
-    <definedName name="項番3" localSheetId="7">#REF!</definedName>
     <definedName name="項番3" localSheetId="8">#REF!</definedName>
     <definedName name="項番3" localSheetId="4">#REF!</definedName>
+    <definedName name="項番3" localSheetId="7">#REF!</definedName>
     <definedName name="項番3" localSheetId="6">#REF!</definedName>
     <definedName name="項番3" localSheetId="5">#REF!</definedName>
     <definedName name="項番3">#REF!</definedName>
@@ -118,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="228">
   <si>
     <t>No</t>
   </si>
@@ -481,10 +482,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Blog</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Comment</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -493,14 +490,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>blog</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Blog</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>title</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -543,10 +532,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Thumbnail Image</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>VARCHAR(100)</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -563,282 +548,322 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>Date Updated</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Yes</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>User ID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>INT(11)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blog 1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>blog 2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Loren ispum…</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Relationship Information (FK Side)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Title Post</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Description Post</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Content Post</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>VARCHAR(64)</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>md5 encrypt</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>VARCHAR(30)</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>avatar</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>Format mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t>date_join</t>
+  </si>
+  <si>
+    <t>Format mm/dd/yyyy hh:mm:ss</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>addreess</t>
+  </si>
+  <si>
+    <t>VARCHAR(200)</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>VARCHAR(50)</t>
+  </si>
+  <si>
+    <t>Format name@name_domail.com</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>63c49caad46ca3e44224962d9c26d781</t>
+  </si>
+  <si>
+    <t>Vu</t>
+  </si>
+  <si>
+    <t>Truong Minh</t>
+  </si>
+  <si>
+    <t>http://k14.vcmedia.vn/k:LJ9BRCA2SwO2i2yoqIMzIMq9QI2QMI/Image/2014/12/ca13-d55f6/man-nhan-voi-bo-anh-ve-loai-cao-trong-mua-dong-lanh-gia.jpg</t>
+  </si>
+  <si>
+    <t>05/29/1976</t>
+  </si>
+  <si>
+    <t>12/22/2014 04:50:21</t>
+  </si>
+  <si>
+    <t>111D Ly Chinh Thang,Q 3</t>
+  </si>
+  <si>
+    <t>Ho Chi Minh</t>
+  </si>
+  <si>
+    <t>vutm@mulodo.com</t>
+  </si>
+  <si>
+    <t>0123.456.78910</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>VARCHAR(250)</t>
+  </si>
+  <si>
+    <t>Date Create</t>
+  </si>
+  <si>
+    <t>date_create</t>
+  </si>
+  <si>
+    <t>Date Update</t>
+  </si>
+  <si>
+    <t>date_update</t>
+  </si>
+  <si>
+    <t>user</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_blog</t>
+  </si>
+  <si>
+    <t>Topping pastry donut. Apple pie sweet marshmallow chocolate bar. Macaroon toffee caramels chocolate bar sweet roll caramels. Jelly beans muffin jujubes gingerbread chocolate gingerbread icing cupcake chupa chups. Icing sugar plum oat cake gummies bonbon cupcake</t>
+  </si>
+  <si>
+    <t>Cheesecake cake chocolate cake cookie candy gummi bears tootsie roll chocolate. Oat cake marzipan chupa chups carrot cake marshmallow sweet roll. Gummies powder brownie cheesecake cupcake bonbon gummi bears gummies topping. Soufflé gummi bears dessert caramels carrot cake marshmallow bear claw gingerbread. Jelly-o pie lemon drops halvah ice cream candy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 = enalble, 0 = disable </t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>1 = Male, 0 = Female</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Date User Create</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Date User Update</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>Date Created</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>date_created</t>
+    <t>created_dt</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Date Updated</t>
+    <t>updated_dt</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>date_updated</t>
+    <t>Post</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Yes</t>
+    <t>post</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>user_id</t>
+    <t>Post ID</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>post_id</t>
+    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>user_id</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>User ID</t>
-  </si>
-  <si>
-    <t>User ID</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>user_id</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>INT(11)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>title</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>blog 1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>blog 2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Loren ispum…</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>DATETIME</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Relationship Information (FK Side)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>user</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Title Post</t>
+    <t>post_id</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Description Post</t>
+    <t>Post</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>Content Post</t>
+    <t>Image Name</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>VARCHAR(64)</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>md5 encrypt</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>VARCHAR(30)</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>Avatar</t>
-  </si>
-  <si>
-    <t>avatar</t>
-  </si>
-  <si>
-    <t>link</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>Birthday</t>
-  </si>
-  <si>
-    <t>birthday</t>
-  </si>
-  <si>
-    <t>DATE</t>
-  </si>
-  <si>
-    <t>Format mm/dd/yyyy</t>
-  </si>
-  <si>
-    <t>Date User Join</t>
-  </si>
-  <si>
-    <t>date_join</t>
-  </si>
-  <si>
-    <t>Format mm/dd/yyyy hh:mm:ss</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>addreess</t>
-  </si>
-  <si>
-    <t>VARCHAR(200)</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>VARCHAR(50)</t>
-  </si>
-  <si>
-    <t>Format name@name_domail.com</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>mobile</t>
-  </si>
-  <si>
-    <t>63c49caad46ca3e44224962d9c26d781</t>
-  </si>
-  <si>
-    <t>Vu</t>
-  </si>
-  <si>
-    <t>Truong Minh</t>
-  </si>
-  <si>
-    <t>http://k14.vcmedia.vn/k:LJ9BRCA2SwO2i2yoqIMzIMq9QI2QMI/Image/2014/12/ca13-d55f6/man-nhan-voi-bo-anh-ve-loai-cao-trong-mua-dong-lanh-gia.jpg</t>
-  </si>
-  <si>
-    <t>05/29/1976</t>
-  </si>
-  <si>
-    <t>12/22/2014 04:50:21</t>
-  </si>
-  <si>
-    <t>111D Ly Chinh Thang,Q 3</t>
-  </si>
-  <si>
-    <t>Ho Chi Minh</t>
-  </si>
-  <si>
-    <t>vutm@mulodo.com</t>
-  </si>
-  <si>
-    <t>0123.456.78910</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>VARCHAR(250)</t>
-  </si>
-  <si>
-    <t>Date Create</t>
-  </si>
-  <si>
-    <t>date_create</t>
-  </si>
-  <si>
-    <t>Date Update</t>
-  </si>
-  <si>
-    <t>date_update</t>
-  </si>
-  <si>
-    <t>1 = Enable, 0 = Disable</t>
-  </si>
-  <si>
-    <t>Blog ID</t>
-  </si>
-  <si>
-    <t>blog_id</t>
-  </si>
-  <si>
-    <t>user</t>
+    <t>comment</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>blog_id</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>user_blog</t>
-  </si>
-  <si>
-    <t>Topping pastry donut. Apple pie sweet marshmallow chocolate bar. Macaroon toffee caramels chocolate bar sweet roll caramels. Jelly beans muffin jujubes gingerbread chocolate gingerbread icing cupcake chupa chups. Icing sugar plum oat cake gummies bonbon cupcake</t>
-  </si>
-  <si>
-    <t>Cheesecake cake chocolate cake cookie candy gummi bears tootsie roll chocolate. Oat cake marzipan chupa chups carrot cake marshmallow sweet roll. Gummies powder brownie cheesecake cupcake bonbon gummi bears gummies topping. Soufflé gummi bears dessert caramels carrot cake marshmallow bear claw gingerbread. Jelly-o pie lemon drops halvah ice cream candy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 = enalble, 0 = disable </t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>TINYINT</t>
-  </si>
-  <si>
-    <t>TINYINT</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>1 = Male, 0 = Female</t>
+    <t>Comment</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1952,7 +1977,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="443">
+  <cellStyleXfs count="444">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1972,6 +1997,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3674,6 +3702,12 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3684,26 +3718,26 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3711,12 +3745,6 @@
     <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3753,20 +3781,26 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3798,9 +3832,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3825,11 +3856,8 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="443">
+  <cellStyles count="444">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -4265,6 +4293,7 @@
     <cellStyle name="Followed Hyperlink" xfId="440" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ハイパーリンク 2" xfId="4"/>
@@ -5518,29 +5547,29 @@
       <c r="L13" s="4"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
-      <c r="O13" s="145"/>
-      <c r="P13" s="145"/>
-      <c r="Q13" s="145"/>
-      <c r="R13" s="145"/>
-      <c r="S13" s="145"/>
-      <c r="T13" s="145"/>
-      <c r="U13" s="145"/>
-      <c r="V13" s="145"/>
-      <c r="W13" s="145"/>
-      <c r="X13" s="145"/>
-      <c r="Y13" s="145"/>
-      <c r="Z13" s="145"/>
-      <c r="AA13" s="145"/>
-      <c r="AB13" s="145"/>
-      <c r="AC13" s="145"/>
-      <c r="AD13" s="145"/>
-      <c r="AE13" s="145"/>
-      <c r="AF13" s="145"/>
-      <c r="AG13" s="145"/>
-      <c r="AH13" s="145"/>
-      <c r="AI13" s="145"/>
-      <c r="AJ13" s="145"/>
-      <c r="AK13" s="145"/>
+      <c r="O13" s="147"/>
+      <c r="P13" s="147"/>
+      <c r="Q13" s="147"/>
+      <c r="R13" s="147"/>
+      <c r="S13" s="147"/>
+      <c r="T13" s="147"/>
+      <c r="U13" s="147"/>
+      <c r="V13" s="147"/>
+      <c r="W13" s="147"/>
+      <c r="X13" s="147"/>
+      <c r="Y13" s="147"/>
+      <c r="Z13" s="147"/>
+      <c r="AA13" s="147"/>
+      <c r="AB13" s="147"/>
+      <c r="AC13" s="147"/>
+      <c r="AD13" s="147"/>
+      <c r="AE13" s="147"/>
+      <c r="AF13" s="147"/>
+      <c r="AG13" s="147"/>
+      <c r="AH13" s="147"/>
+      <c r="AI13" s="147"/>
+      <c r="AJ13" s="147"/>
+      <c r="AK13" s="147"/>
       <c r="AL13" s="4"/>
       <c r="AM13" s="4"/>
       <c r="AN13" s="4"/>
@@ -5572,29 +5601,29 @@
       <c r="L14" s="4"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
-      <c r="O14" s="145"/>
-      <c r="P14" s="145"/>
-      <c r="Q14" s="145"/>
-      <c r="R14" s="145"/>
-      <c r="S14" s="145"/>
-      <c r="T14" s="145"/>
-      <c r="U14" s="145"/>
-      <c r="V14" s="145"/>
-      <c r="W14" s="145"/>
-      <c r="X14" s="145"/>
-      <c r="Y14" s="145"/>
-      <c r="Z14" s="145"/>
-      <c r="AA14" s="145"/>
-      <c r="AB14" s="145"/>
-      <c r="AC14" s="145"/>
-      <c r="AD14" s="145"/>
-      <c r="AE14" s="145"/>
-      <c r="AF14" s="145"/>
-      <c r="AG14" s="145"/>
-      <c r="AH14" s="145"/>
-      <c r="AI14" s="145"/>
-      <c r="AJ14" s="145"/>
-      <c r="AK14" s="145"/>
+      <c r="O14" s="147"/>
+      <c r="P14" s="147"/>
+      <c r="Q14" s="147"/>
+      <c r="R14" s="147"/>
+      <c r="S14" s="147"/>
+      <c r="T14" s="147"/>
+      <c r="U14" s="147"/>
+      <c r="V14" s="147"/>
+      <c r="W14" s="147"/>
+      <c r="X14" s="147"/>
+      <c r="Y14" s="147"/>
+      <c r="Z14" s="147"/>
+      <c r="AA14" s="147"/>
+      <c r="AB14" s="147"/>
+      <c r="AC14" s="147"/>
+      <c r="AD14" s="147"/>
+      <c r="AE14" s="147"/>
+      <c r="AF14" s="147"/>
+      <c r="AG14" s="147"/>
+      <c r="AH14" s="147"/>
+      <c r="AI14" s="147"/>
+      <c r="AJ14" s="147"/>
+      <c r="AK14" s="147"/>
       <c r="AL14" s="4"/>
       <c r="AM14" s="4"/>
       <c r="AN14" s="4"/>
@@ -5622,43 +5651,43 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="146" t="s">
+      <c r="K15" s="148" t="s">
         <v>112</v>
       </c>
-      <c r="L15" s="146"/>
-      <c r="M15" s="146"/>
-      <c r="N15" s="146"/>
-      <c r="O15" s="146"/>
-      <c r="P15" s="146"/>
-      <c r="Q15" s="146"/>
-      <c r="R15" s="146"/>
-      <c r="S15" s="146"/>
-      <c r="T15" s="146"/>
-      <c r="U15" s="146"/>
-      <c r="V15" s="146"/>
-      <c r="W15" s="146"/>
-      <c r="X15" s="146"/>
-      <c r="Y15" s="146"/>
-      <c r="Z15" s="146"/>
-      <c r="AA15" s="146"/>
-      <c r="AB15" s="146"/>
-      <c r="AC15" s="146"/>
-      <c r="AD15" s="146"/>
-      <c r="AE15" s="146"/>
-      <c r="AF15" s="146"/>
-      <c r="AG15" s="146"/>
-      <c r="AH15" s="146"/>
-      <c r="AI15" s="146"/>
-      <c r="AJ15" s="146"/>
-      <c r="AK15" s="146"/>
-      <c r="AL15" s="146"/>
-      <c r="AM15" s="146"/>
-      <c r="AN15" s="146"/>
-      <c r="AO15" s="146"/>
-      <c r="AP15" s="146"/>
-      <c r="AQ15" s="146"/>
-      <c r="AR15" s="146"/>
-      <c r="AS15" s="146"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="148"/>
+      <c r="N15" s="148"/>
+      <c r="O15" s="148"/>
+      <c r="P15" s="148"/>
+      <c r="Q15" s="148"/>
+      <c r="R15" s="148"/>
+      <c r="S15" s="148"/>
+      <c r="T15" s="148"/>
+      <c r="U15" s="148"/>
+      <c r="V15" s="148"/>
+      <c r="W15" s="148"/>
+      <c r="X15" s="148"/>
+      <c r="Y15" s="148"/>
+      <c r="Z15" s="148"/>
+      <c r="AA15" s="148"/>
+      <c r="AB15" s="148"/>
+      <c r="AC15" s="148"/>
+      <c r="AD15" s="148"/>
+      <c r="AE15" s="148"/>
+      <c r="AF15" s="148"/>
+      <c r="AG15" s="148"/>
+      <c r="AH15" s="148"/>
+      <c r="AI15" s="148"/>
+      <c r="AJ15" s="148"/>
+      <c r="AK15" s="148"/>
+      <c r="AL15" s="148"/>
+      <c r="AM15" s="148"/>
+      <c r="AN15" s="148"/>
+      <c r="AO15" s="148"/>
+      <c r="AP15" s="148"/>
+      <c r="AQ15" s="148"/>
+      <c r="AR15" s="148"/>
+      <c r="AS15" s="148"/>
       <c r="AT15" s="4"/>
       <c r="AU15" s="4"/>
       <c r="AV15" s="4"/>
@@ -5678,41 +5707,41 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="146"/>
-      <c r="M16" s="146"/>
-      <c r="N16" s="146"/>
-      <c r="O16" s="146"/>
-      <c r="P16" s="146"/>
-      <c r="Q16" s="146"/>
-      <c r="R16" s="146"/>
-      <c r="S16" s="146"/>
-      <c r="T16" s="146"/>
-      <c r="U16" s="146"/>
-      <c r="V16" s="146"/>
-      <c r="W16" s="146"/>
-      <c r="X16" s="146"/>
-      <c r="Y16" s="146"/>
-      <c r="Z16" s="146"/>
-      <c r="AA16" s="146"/>
-      <c r="AB16" s="146"/>
-      <c r="AC16" s="146"/>
-      <c r="AD16" s="146"/>
-      <c r="AE16" s="146"/>
-      <c r="AF16" s="146"/>
-      <c r="AG16" s="146"/>
-      <c r="AH16" s="146"/>
-      <c r="AI16" s="146"/>
-      <c r="AJ16" s="146"/>
-      <c r="AK16" s="146"/>
-      <c r="AL16" s="146"/>
-      <c r="AM16" s="146"/>
-      <c r="AN16" s="146"/>
-      <c r="AO16" s="146"/>
-      <c r="AP16" s="146"/>
-      <c r="AQ16" s="146"/>
-      <c r="AR16" s="146"/>
-      <c r="AS16" s="146"/>
+      <c r="K16" s="148"/>
+      <c r="L16" s="148"/>
+      <c r="M16" s="148"/>
+      <c r="N16" s="148"/>
+      <c r="O16" s="148"/>
+      <c r="P16" s="148"/>
+      <c r="Q16" s="148"/>
+      <c r="R16" s="148"/>
+      <c r="S16" s="148"/>
+      <c r="T16" s="148"/>
+      <c r="U16" s="148"/>
+      <c r="V16" s="148"/>
+      <c r="W16" s="148"/>
+      <c r="X16" s="148"/>
+      <c r="Y16" s="148"/>
+      <c r="Z16" s="148"/>
+      <c r="AA16" s="148"/>
+      <c r="AB16" s="148"/>
+      <c r="AC16" s="148"/>
+      <c r="AD16" s="148"/>
+      <c r="AE16" s="148"/>
+      <c r="AF16" s="148"/>
+      <c r="AG16" s="148"/>
+      <c r="AH16" s="148"/>
+      <c r="AI16" s="148"/>
+      <c r="AJ16" s="148"/>
+      <c r="AK16" s="148"/>
+      <c r="AL16" s="148"/>
+      <c r="AM16" s="148"/>
+      <c r="AN16" s="148"/>
+      <c r="AO16" s="148"/>
+      <c r="AP16" s="148"/>
+      <c r="AQ16" s="148"/>
+      <c r="AR16" s="148"/>
+      <c r="AS16" s="148"/>
       <c r="AT16" s="4"/>
       <c r="AU16" s="4"/>
       <c r="AV16" s="4"/>
@@ -6301,14 +6330,14 @@
       <c r="AK27" s="4"/>
       <c r="AL27" s="4"/>
       <c r="AM27" s="7"/>
-      <c r="AN27" s="147" t="s">
+      <c r="AN27" s="149" t="s">
         <v>113</v>
       </c>
-      <c r="AO27" s="147"/>
-      <c r="AP27" s="147"/>
-      <c r="AQ27" s="147"/>
-      <c r="AR27" s="147"/>
-      <c r="AS27" s="147"/>
+      <c r="AO27" s="149"/>
+      <c r="AP27" s="149"/>
+      <c r="AQ27" s="149"/>
+      <c r="AR27" s="149"/>
+      <c r="AS27" s="149"/>
       <c r="AT27" s="12"/>
       <c r="AU27" s="12"/>
       <c r="AV27" s="12"/>
@@ -7067,11 +7096,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="12" thickBot="1">
-      <c r="A1" s="148" t="s">
+      <c r="A1" s="150" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="148"/>
-      <c r="C1" s="148"/>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
     </row>
     <row r="2" spans="1:3" ht="12" thickBot="1">
       <c r="A2" s="118" t="s">
@@ -7101,11 +7130,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>118</v>
+        <v>224</v>
       </c>
       <c r="C4" s="137" t="str">
-        <f>HYPERLINK("#blog","blog")</f>
-        <v>blog</v>
+        <f>HYPERLINK("#post","post")</f>
+        <v>post</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17">
@@ -7114,7 +7143,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="137" t="str">
         <f>HYPERLINK("#comment","comment")</f>
@@ -7332,11 +7361,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U38"/>
+  <dimension ref="A1:U39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
-    </sheetView>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -7365,67 +7392,67 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="149"/>
-      <c r="G2" s="153"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:21" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:21" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:21" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="176" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:21" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="176" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="152"/>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:21" ht="13">
       <c r="B7" s="160" t="s">
@@ -7501,34 +7528,34 @@
         <v>111</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="M13" s="128" t="s">
+        <v>164</v>
+      </c>
+      <c r="N13" s="128" t="s">
+        <v>166</v>
+      </c>
+      <c r="O13" s="128" t="s">
+        <v>169</v>
+      </c>
+      <c r="P13" s="128" t="s">
         <v>171</v>
       </c>
-      <c r="N13" s="128" t="s">
-        <v>173</v>
-      </c>
-      <c r="O13" s="128" t="s">
-        <v>176</v>
-      </c>
-      <c r="P13" s="128" t="s">
-        <v>178</v>
-      </c>
       <c r="Q13" s="128" t="s">
+        <v>174</v>
+      </c>
+      <c r="R13" s="128" t="s">
+        <v>197</v>
+      </c>
+      <c r="S13" s="128" t="s">
+        <v>180</v>
+      </c>
+      <c r="T13" s="128" t="s">
         <v>182</v>
       </c>
-      <c r="R13" s="128" t="s">
-        <v>205</v>
-      </c>
-      <c r="S13" s="128" t="s">
-        <v>188</v>
-      </c>
-      <c r="T13" s="128" t="s">
-        <v>190</v>
-      </c>
       <c r="U13" s="128" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="17">
@@ -7559,37 +7586,37 @@
         <v>108</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="L14" s="13" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="M14" s="13" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="N14" s="136" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="O14" s="13">
         <v>1</v>
       </c>
       <c r="P14" s="127" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="Q14" s="127" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="R14" s="127" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="S14" s="13" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="T14" s="136" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="U14" s="18" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="17">
@@ -7604,7 +7631,7 @@
         <v>105</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -7621,24 +7648,24 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A23" si="0">A15+1</f>
+        <f t="shared" ref="A16:A24" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C16" s="65" t="s">
         <v>111</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -7648,13 +7675,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
@@ -7669,13 +7696,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
@@ -7690,20 +7717,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D19" s="65" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -7712,22 +7739,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="187">
+      <c r="F20" s="145">
         <v>1</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>222</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -7736,260 +7763,282 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="59">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>A20+1</f>
+        <v>8</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>181</v>
+        <v>210</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>182</v>
+        <v>211</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F22" s="67"/>
       <c r="G22" s="106" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" s="59">
+        <f>A21+1</f>
+        <v>9</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>212</v>
+      </c>
+      <c r="C23" s="65" t="s">
+        <v>213</v>
+      </c>
+      <c r="D23" s="65" t="s">
+        <v>148</v>
+      </c>
+      <c r="E23" s="66" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="67"/>
+      <c r="G23" s="106" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="59">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B23" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>185</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="66" t="s">
+      <c r="B24" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106"/>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="139">
-        <v>11</v>
-      </c>
-      <c r="B24" s="140" t="s">
-        <v>187</v>
-      </c>
-      <c r="C24" s="141" t="s">
-        <v>188</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>169</v>
-      </c>
-      <c r="E24" s="142" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="143"/>
-      <c r="G24" s="144"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="106"/>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" s="139">
+        <v>11</v>
+      </c>
+      <c r="B25" s="140" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="141" t="s">
+        <v>180</v>
+      </c>
+      <c r="D25" s="65" t="s">
+        <v>162</v>
+      </c>
+      <c r="E25" s="142" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="143"/>
+      <c r="G25" s="144"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="139">
         <v>12</v>
       </c>
-      <c r="B25" s="140" t="s">
-        <v>189</v>
-      </c>
-      <c r="C25" s="141" t="s">
-        <v>190</v>
-      </c>
-      <c r="D25" s="65" t="s">
-        <v>191</v>
-      </c>
-      <c r="E25" s="142" t="s">
+      <c r="B26" s="140" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="141" t="s">
+        <v>182</v>
+      </c>
+      <c r="D26" s="65" t="s">
+        <v>183</v>
+      </c>
+      <c r="E26" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="143"/>
-      <c r="G25" s="144" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="12" thickBot="1">
-      <c r="A26" s="70">
+      <c r="F26" s="143"/>
+      <c r="G26" s="144" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="12" thickBot="1">
+      <c r="A27" s="70">
         <v>13</v>
       </c>
-      <c r="B26" s="131" t="s">
-        <v>193</v>
-      </c>
-      <c r="C26" s="132" t="s">
-        <v>194</v>
-      </c>
-      <c r="D26" s="132" t="s">
+      <c r="B27" s="131" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" s="132" t="s">
+        <v>186</v>
+      </c>
+      <c r="D27" s="132" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="133" t="s">
+      <c r="E27" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="F26" s="135"/>
-      <c r="G26" s="134"/>
-    </row>
-    <row r="28" spans="1:8" ht="12" thickBot="1">
-      <c r="A28" s="1" t="s">
+      <c r="F27" s="135"/>
+      <c r="G27" s="134"/>
+    </row>
+    <row r="29" spans="1:8" ht="12" thickBot="1">
+      <c r="A29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
-      <c r="A29" s="29" t="s">
+    <row r="30" spans="1:8">
+      <c r="A30" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B30" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="156" t="s">
+      <c r="C30" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="157"/>
-      <c r="E29" s="34" t="s">
+      <c r="D30" s="159"/>
+      <c r="E30" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F30" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G29" s="35" t="s">
+      <c r="G30" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13">
-      <c r="A30" s="14">
+    <row r="31" spans="1:8" ht="13">
+      <c r="A31" s="14">
         <v>1</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="170" t="s">
+      <c r="C31" s="170" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="171"/>
-      <c r="E30" s="46" t="s">
+      <c r="D31" s="171"/>
+      <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F31" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" spans="1:8" ht="13" customHeight="1">
-      <c r="A31" s="57">
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:8" ht="13" customHeight="1">
+      <c r="A32" s="57">
         <v>2</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="175"/>
-      <c r="D31" s="176"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="53"/>
-    </row>
-    <row r="32" spans="1:8" ht="13" customHeight="1" thickBot="1">
-      <c r="A32" s="56">
+      <c r="B32" s="51"/>
+      <c r="C32" s="156"/>
+      <c r="D32" s="157"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="53"/>
+    </row>
+    <row r="33" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A33" s="56">
         <v>3</v>
       </c>
-      <c r="B32" s="54"/>
-      <c r="C32" s="173"/>
-      <c r="D32" s="174"/>
-      <c r="E32" s="58"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="55"/>
-    </row>
-    <row r="34" spans="1:7" ht="12" thickBot="1">
-      <c r="A34" s="1" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="154"/>
+      <c r="D33" s="155"/>
+      <c r="E33" s="58"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="55"/>
+    </row>
+    <row r="35" spans="1:7" ht="12" thickBot="1">
+      <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="14" thickBot="1">
-      <c r="A35" s="36" t="s">
+    <row r="36" spans="1:7" ht="14" thickBot="1">
+      <c r="A36" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="158" t="s">
+      <c r="C36" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D35" s="159"/>
-      <c r="E35" s="158" t="s">
+      <c r="D36" s="152"/>
+      <c r="E36" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="172"/>
-      <c r="G35" s="38" t="s">
+      <c r="F36" s="153"/>
+      <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="12" thickBot="1">
-      <c r="A37" s="1" t="s">
+    <row r="38" spans="1:7" ht="12" thickBot="1">
+      <c r="A38" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="14" thickBot="1">
-      <c r="A38" s="36" t="s">
+    <row r="39" spans="1:7" ht="14" thickBot="1">
+      <c r="A39" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="158" t="s">
+      <c r="C39" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="159"/>
-      <c r="E38" s="158" t="s">
+      <c r="D39" s="152"/>
+      <c r="E39" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="172"/>
-      <c r="G38" s="38" t="s">
+      <c r="F39" s="153"/>
+      <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
@@ -8041,69 +8090,69 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="153"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="176" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="176" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="152"/>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:11" ht="13">
       <c r="B7" s="160" t="s">
@@ -8359,10 +8408,10 @@
       <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="156" t="s">
+      <c r="C24" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="157"/>
+      <c r="D24" s="159"/>
       <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
@@ -8397,10 +8446,10 @@
         <v>2</v>
       </c>
       <c r="B26" s="54"/>
-      <c r="C26" s="179" t="s">
+      <c r="C26" s="181" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="180"/>
+      <c r="D26" s="182"/>
       <c r="E26" s="58"/>
       <c r="F26" s="58" t="s">
         <v>3</v>
@@ -8419,14 +8468,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="158" t="s">
+      <c r="C29" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="159"/>
-      <c r="E29" s="158" t="s">
+      <c r="D29" s="152"/>
+      <c r="E29" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="172"/>
+      <c r="F29" s="153"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8443,14 +8492,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="158" t="s">
+      <c r="C32" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="159"/>
-      <c r="E32" s="158" t="s">
+      <c r="D32" s="152"/>
+      <c r="E32" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="172"/>
+      <c r="F32" s="153"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8460,29 +8509,20 @@
         <v>1</v>
       </c>
       <c r="B33" s="26"/>
-      <c r="C33" s="177" t="s">
+      <c r="C33" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="178"/>
-      <c r="E33" s="179" t="s">
+      <c r="D33" s="180"/>
+      <c r="E33" s="181" t="s">
         <v>47</v>
       </c>
-      <c r="F33" s="180"/>
+      <c r="F33" s="182"/>
       <c r="G33" s="28" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8495,6 +8535,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8542,69 +8591,69 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="149" t="s">
+      <c r="F2" s="172" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="153"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="151" t="s">
+      <c r="F3" s="176" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="176" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="176" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="152"/>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:7" ht="13">
       <c r="B7" s="160" t="s">
@@ -8745,10 +8794,10 @@
       <c r="B19" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="156" t="s">
+      <c r="C19" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="157"/>
+      <c r="D19" s="159"/>
       <c r="E19" s="34" t="s">
         <v>33</v>
       </c>
@@ -8783,10 +8832,10 @@
         <v>2</v>
       </c>
       <c r="B21" s="26"/>
-      <c r="C21" s="177" t="s">
+      <c r="C21" s="179" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="178"/>
+      <c r="D21" s="180"/>
       <c r="E21" s="45"/>
       <c r="F21" s="45" t="s">
         <v>3</v>
@@ -8805,14 +8854,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="158" t="s">
+      <c r="C24" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="159"/>
-      <c r="E24" s="158" t="s">
+      <c r="D24" s="152"/>
+      <c r="E24" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="172"/>
+      <c r="F24" s="153"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -8829,14 +8878,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="158" t="s">
+      <c r="C27" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="159"/>
-      <c r="E27" s="158" t="s">
+      <c r="D27" s="152"/>
+      <c r="E27" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="172"/>
+      <c r="F27" s="153"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -8846,23 +8895,14 @@
         <v>1</v>
       </c>
       <c r="B28" s="26"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="178"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="180"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="180"/>
+      <c r="E28" s="181"/>
+      <c r="F28" s="182"/>
       <c r="G28" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8875,6 +8915,15 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8922,69 +8971,69 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="183" t="s">
+      <c r="F2" s="185" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="184"/>
+      <c r="G2" s="186"/>
     </row>
     <row r="3" spans="1:14" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="174" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
+      <c r="C5" s="176" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="152"/>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
+      <c r="C6" s="176" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="152"/>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:14" ht="13">
       <c r="B7" s="160" t="s">
@@ -9234,10 +9283,10 @@
       <c r="B21" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="156" t="s">
+      <c r="C21" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="157"/>
+      <c r="D21" s="159"/>
       <c r="E21" s="34" t="s">
         <v>33</v>
       </c>
@@ -9284,10 +9333,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="175" t="s">
+      <c r="C23" s="156" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="176"/>
+      <c r="D23" s="157"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -9305,10 +9354,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="26"/>
-      <c r="C24" s="177" t="s">
+      <c r="C24" s="179" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="178"/>
+      <c r="D24" s="180"/>
       <c r="E24" s="45"/>
       <c r="F24" s="45" t="s">
         <v>3</v>
@@ -9347,14 +9396,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="158" t="s">
+      <c r="C27" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="159"/>
-      <c r="E27" s="158" t="s">
+      <c r="D27" s="152"/>
+      <c r="E27" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="172"/>
+      <c r="F27" s="153"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -9391,14 +9440,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="158" t="s">
+      <c r="C30" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="159"/>
-      <c r="E30" s="158" t="s">
+      <c r="D30" s="152"/>
+      <c r="E30" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="172"/>
+      <c r="F30" s="153"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -9418,10 +9467,10 @@
         <v>76</v>
       </c>
       <c r="D31" s="171"/>
-      <c r="E31" s="175" t="s">
+      <c r="E31" s="156" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="176"/>
+      <c r="F31" s="157"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -9437,14 +9486,14 @@
         <v>2</v>
       </c>
       <c r="B32" s="26"/>
-      <c r="C32" s="181" t="s">
+      <c r="C32" s="183" t="s">
         <v>52</v>
       </c>
-      <c r="D32" s="182"/>
-      <c r="E32" s="179" t="s">
+      <c r="D32" s="184"/>
+      <c r="E32" s="181" t="s">
         <v>69</v>
       </c>
-      <c r="F32" s="180"/>
+      <c r="F32" s="182"/>
       <c r="G32" s="55" t="s">
         <v>52</v>
       </c>
@@ -9497,6 +9546,14 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -9513,14 +9570,6 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9544,8 +9593,8 @@
   </sheetPr>
   <dimension ref="A1:S37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9575,67 +9624,67 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="149"/>
-      <c r="G2" s="153"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="152"/>
+      <c r="C5" s="176" t="s">
+        <v>217</v>
+      </c>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="152"/>
+      <c r="C6" s="176" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:19" ht="13">
       <c r="B7" s="160" t="s">
@@ -9705,10 +9754,10 @@
         <v>109</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="L13" s="128" t="s">
         <v>114</v>
@@ -9752,10 +9801,10 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="N14" s="136"/>
       <c r="P14" s="127"/>
@@ -9768,13 +9817,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -9786,10 +9835,10 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="K15" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="N15" s="136"/>
       <c r="P15" s="127"/>
@@ -9802,16 +9851,16 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E16" s="66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117"/>
@@ -9823,16 +9872,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="E17" s="66" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117"/>
@@ -9843,16 +9892,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>134</v>
+        <v>225</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D18" s="129" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E18" s="66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106"/>
@@ -9863,22 +9912,22 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="196" t="s">
-        <v>138</v>
+        <v>125</v>
+      </c>
+      <c r="F19" s="146" t="s">
+        <v>134</v>
       </c>
       <c r="G19" s="106" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -9887,20 +9936,20 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>139</v>
+        <v>214</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E20" s="66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F20" s="67"/>
       <c r="G20" s="106" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9909,20 +9958,20 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="D21" s="65" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="E21" s="66" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -9931,16 +9980,16 @@
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="E22" s="66" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F22" s="67"/>
       <c r="G22" s="106"/>
@@ -9981,10 +10030,10 @@
       <c r="B27" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="156" t="s">
+      <c r="C27" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="157"/>
+      <c r="D27" s="159"/>
       <c r="E27" s="34" t="s">
         <v>33</v>
       </c>
@@ -10019,8 +10068,8 @@
         <v>2</v>
       </c>
       <c r="B29" s="51"/>
-      <c r="C29" s="175"/>
-      <c r="D29" s="176"/>
+      <c r="C29" s="156"/>
+      <c r="D29" s="157"/>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
       <c r="G29" s="53"/>
@@ -10030,15 +10079,15 @@
         <v>3</v>
       </c>
       <c r="B30" s="54"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="174"/>
+      <c r="C30" s="154"/>
+      <c r="D30" s="155"/>
       <c r="E30" s="58"/>
       <c r="F30" s="58"/>
       <c r="G30" s="55"/>
     </row>
     <row r="32" spans="1:7" ht="12" thickBot="1">
       <c r="A32" s="1" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14" thickBot="1">
@@ -10048,14 +10097,14 @@
       <c r="B33" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="158" t="s">
+      <c r="C33" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="159"/>
-      <c r="E33" s="158" t="s">
+      <c r="D33" s="152"/>
+      <c r="E33" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="172"/>
+      <c r="F33" s="153"/>
       <c r="G33" s="38" t="s">
         <v>38</v>
       </c>
@@ -10066,15 +10115,15 @@
       </c>
       <c r="B34" s="19"/>
       <c r="C34" s="170" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D34" s="171"/>
-      <c r="E34" s="185" t="s">
-        <v>159</v>
-      </c>
-      <c r="F34" s="186"/>
+      <c r="E34" s="187" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="188"/>
       <c r="G34" s="20" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="12" thickBot="1">
@@ -10089,20 +10138,30 @@
       <c r="B37" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="158" t="s">
+      <c r="C37" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D37" s="159"/>
-      <c r="E37" s="158" t="s">
+      <c r="D37" s="152"/>
+      <c r="E37" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="172"/>
+      <c r="F37" s="153"/>
       <c r="G37" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10115,16 +10174,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10146,11 +10195,9 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S39"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -10172,74 +10219,74 @@
   <sheetData>
     <row r="1" spans="1:19" ht="12" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="13">
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="149" t="s">
+      <c r="C2" s="172" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="150"/>
+      <c r="D2" s="177"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="149"/>
-      <c r="G2" s="153"/>
+      <c r="F2" s="172"/>
+      <c r="G2" s="173"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="151"/>
-      <c r="D3" s="152"/>
+      <c r="C3" s="176"/>
+      <c r="D3" s="178"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="154" t="s">
+      <c r="F3" s="174" t="s">
         <v>116</v>
       </c>
-      <c r="G3" s="155"/>
+      <c r="G3" s="175"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="176" t="s">
         <v>117</v>
       </c>
-      <c r="D4" s="152"/>
+      <c r="D4" s="178"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="151"/>
-      <c r="G4" s="155"/>
+      <c r="F4" s="176"/>
+      <c r="G4" s="175"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="151" t="s">
-        <v>103</v>
-      </c>
-      <c r="D5" s="152"/>
+      <c r="C5" s="176" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="178"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="155"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="175"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="151" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="152"/>
+      <c r="C6" s="176" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="178"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="151"/>
-      <c r="G6" s="155"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="175"/>
     </row>
     <row r="7" spans="1:19" ht="13">
       <c r="B7" s="160" t="s">
@@ -10309,22 +10356,22 @@
         <v>109</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="M13" s="128" t="s">
         <v>6</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="O13" s="128" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="P13" s="128"/>
       <c r="Q13" s="128"/>
@@ -10356,13 +10403,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="K14" s="127" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L14" s="127" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="M14" s="13">
         <v>1</v>
@@ -10386,10 +10433,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10401,13 +10448,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="K15" s="127" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="L15" s="127" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="M15" s="13">
         <v>0</v>
@@ -10428,20 +10475,20 @@
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="106" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -10451,20 +10498,20 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D17" s="65" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="106" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -10472,65 +10519,54 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>6</v>
+        <v>137</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>221</v>
+        <v>53</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="187">
-        <v>1</v>
-      </c>
-      <c r="G18" s="106" t="s">
-        <v>211</v>
-      </c>
+      <c r="F18" s="67"/>
+      <c r="G18" s="106"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="59">
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>146</v>
+        <v>219</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>144</v>
-      </c>
-      <c r="D19" s="65" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="129" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="67"/>
+      <c r="F19" s="138"/>
       <c r="G19" s="106"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="59">
+        <f t="shared" ref="A20:A23" si="1">A19+1</f>
         <v>7</v>
       </c>
-      <c r="B20" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C20" s="65" t="s">
-        <v>213</v>
-      </c>
-      <c r="D20" s="129" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" s="66" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="138"/>
+      <c r="B20" s="63"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="67"/>
       <c r="G20" s="106"/>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" s="59">
-        <f t="shared" ref="A21:A24" si="1">A20+1</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B21" s="63"/>
@@ -10552,119 +10588,124 @@
       <c r="F22" s="67"/>
       <c r="G22" s="106"/>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="59">
+    <row r="23" spans="1:7" ht="12" thickBot="1">
+      <c r="A23" s="70">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106"/>
-    </row>
-    <row r="24" spans="1:7" ht="12" thickBot="1">
-      <c r="A24" s="70">
-        <f t="shared" si="1"/>
-        <v>11</v>
-      </c>
-      <c r="B24" s="131"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="134"/>
-    </row>
-    <row r="26" spans="1:7" ht="12" thickBot="1">
-      <c r="A26" s="1" t="s">
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="134"/>
+    </row>
+    <row r="25" spans="1:7" ht="12" thickBot="1">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="29" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="156" t="s">
+      <c r="C26" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="157"/>
-      <c r="E27" s="34" t="s">
+      <c r="D26" s="159"/>
+      <c r="E26" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G26" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13">
-      <c r="A28" s="14">
+    <row r="27" spans="1:7" ht="13">
+      <c r="A27" s="14">
         <v>1</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="170" t="s">
+      <c r="C27" s="170" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="171"/>
-      <c r="E28" s="46" t="s">
+      <c r="D27" s="171"/>
+      <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F27" s="46" t="s">
         <v>3</v>
       </c>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="13" customHeight="1">
+      <c r="A28" s="57">
+        <v>2</v>
+      </c>
+      <c r="B28" s="51"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:7" ht="13" customHeight="1">
-      <c r="A29" s="57">
-        <v>2</v>
-      </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="175"/>
-      <c r="D29" s="176"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:7" ht="13" customHeight="1" thickBot="1">
-      <c r="A30" s="56">
+    <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A29" s="56">
         <v>3</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="173"/>
-      <c r="D30" s="174"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="12" thickBot="1">
-      <c r="A32" s="1" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="155"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="55"/>
+    </row>
+    <row r="31" spans="1:7" ht="12" thickBot="1">
+      <c r="A31" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="14" thickBot="1">
-      <c r="A33" s="36" t="s">
+    <row r="32" spans="1:7" ht="14" thickBot="1">
+      <c r="A32" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="158" t="s">
+      <c r="C32" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="159"/>
-      <c r="E33" s="158" t="s">
+      <c r="D32" s="152"/>
+      <c r="E32" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="172"/>
-      <c r="G33" s="38" t="s">
+      <c r="F32" s="153"/>
+      <c r="G32" s="38" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="14">
+        <v>1</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="187" t="s">
+        <v>221</v>
+      </c>
+      <c r="D33" s="188"/>
+      <c r="E33" s="191" t="s">
+        <v>203</v>
+      </c>
+      <c r="F33" s="192"/>
+      <c r="G33" s="20" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -10672,96 +10713,81 @@
         <v>1</v>
       </c>
       <c r="B34" s="19"/>
-      <c r="C34" s="185" t="s">
-        <v>215</v>
-      </c>
-      <c r="D34" s="186"/>
-      <c r="E34" s="190" t="s">
-        <v>214</v>
-      </c>
-      <c r="F34" s="191"/>
+      <c r="C34" s="189" t="s">
+        <v>223</v>
+      </c>
+      <c r="D34" s="190"/>
+      <c r="E34" s="193" t="s">
+        <v>218</v>
+      </c>
+      <c r="F34" s="194"/>
       <c r="G34" s="20" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="14">
-        <v>1</v>
-      </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="188" t="s">
-        <v>215</v>
-      </c>
-      <c r="D35" s="189"/>
-      <c r="E35" s="192" t="s">
-        <v>121</v>
-      </c>
-      <c r="F35" s="193"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="1:7" ht="14" customHeight="1" thickBot="1">
-      <c r="A36" s="56">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14" customHeight="1" thickBot="1">
+      <c r="A35" s="56">
         <v>3</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="173"/>
-      <c r="D36" s="174"/>
-      <c r="E36" s="194"/>
-      <c r="F36" s="195"/>
-      <c r="G36" s="55"/>
+      <c r="B35" s="54"/>
+      <c r="C35" s="154"/>
+      <c r="D35" s="155"/>
+      <c r="E35" s="195"/>
+      <c r="F35" s="196"/>
+      <c r="G35" s="55"/>
+    </row>
+    <row r="37" spans="1:7" ht="12" thickBot="1">
+      <c r="A37" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="38" spans="1:7" ht="12" thickBot="1">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="12" thickBot="1">
-      <c r="A39" s="36" t="s">
+      <c r="A38" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B38" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="158" t="s">
+      <c r="C38" s="151" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="159"/>
-      <c r="E39" s="158" t="s">
+      <c r="D38" s="152"/>
+      <c r="E38" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="159"/>
-      <c r="G39" s="38" t="s">
+      <c r="F38" s="152"/>
+      <c r="G38" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="F4:G4"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
move date to end of table, remove on update
</commit_message>
<xml_diff>
--- a/php/tam-v.anh/doc/detail_design/db/MiniBlog_Database_Design.xlsx
+++ b/php/tam-v.anh/doc/detail_design/db/MiniBlog_Database_Design.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27200" windowHeight="17040" tabRatio="818" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="11" r:id="rId1"/>
@@ -119,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="237">
   <si>
     <t>No</t>
   </si>
@@ -466,10 +466,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>...</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Mini Blog System</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -684,9 +680,6 @@
     <t>Format mm/dd/yyyy</t>
   </si>
   <si>
-    <t>date_join</t>
-  </si>
-  <si>
     <t>Format mm/dd/yyyy hh:mm:ss</t>
   </si>
   <si>
@@ -762,22 +755,13 @@
     <t>Date Create</t>
   </si>
   <si>
-    <t>date_create</t>
-  </si>
-  <si>
     <t>Date Update</t>
-  </si>
-  <si>
-    <t>date_update</t>
   </si>
   <si>
     <t>user</t>
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>user_blog</t>
-  </si>
-  <si>
     <t>Topping pastry donut. Apple pie sweet marshmallow chocolate bar. Macaroon toffee caramels chocolate bar sweet roll caramels. Jelly beans muffin jujubes gingerbread chocolate gingerbread icing cupcake chupa chups. Icing sugar plum oat cake gummies bonbon cupcake</t>
   </si>
   <si>
@@ -864,6 +848,62 @@
   </si>
   <si>
     <t>Comment</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>image</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>status</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>image1.jpg</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Loren ispum…</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>user_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>post_id</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>created_dt</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>updated_dt</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1977,7 +2017,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="444">
+  <cellStyleXfs count="462">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3307,8 +3347,62 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="212">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3718,12 +3812,75 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3739,69 +3896,6 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3856,8 +3950,53 @@
     <xf numFmtId="49" fontId="14" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="444">
+  <cellStyles count="462">
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
@@ -4294,6 +4433,24 @@
     <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="442" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="444" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="446" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="448" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="450" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="452" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="454" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="456" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="458" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="460" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="ハイパーリンク 2" xfId="4"/>
@@ -7084,7 +7241,7 @@
   </sheetPr>
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -7130,7 +7287,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="123" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C4" s="137" t="str">
         <f>HYPERLINK("#post","post")</f>
@@ -7143,7 +7300,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="123" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="137" t="str">
         <f>HYPERLINK("#comment","comment")</f>
@@ -7361,9 +7518,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U39"/>
+  <dimension ref="A1:V39"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView topLeftCell="M1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="S16" sqref="S16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -7378,117 +7537,120 @@
     <col min="12" max="12" width="12.6640625" style="13" customWidth="1"/>
     <col min="13" max="13" width="12.5" style="13" customWidth="1"/>
     <col min="14" max="15" width="19.33203125" style="13" customWidth="1"/>
-    <col min="16" max="17" width="17" style="13" customWidth="1"/>
-    <col min="18" max="18" width="15.5" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="13"/>
+    <col min="16" max="16" width="17" style="13" customWidth="1"/>
+    <col min="17" max="17" width="15.5" style="13" customWidth="1"/>
+    <col min="18" max="19" width="8.83203125" style="13"/>
+    <col min="20" max="20" width="14" style="13" customWidth="1"/>
+    <col min="21" max="22" width="13.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="12" thickBot="1">
+    <row r="1" spans="1:22" ht="12" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="13">
+    <row r="2" spans="1:22" ht="13">
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="177"/>
+      <c r="C2" s="151" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="172"/>
-      <c r="G2" s="173"/>
-    </row>
-    <row r="3" spans="1:21" ht="13">
+      <c r="F2" s="151"/>
+      <c r="G2" s="155"/>
+    </row>
+    <row r="3" spans="1:22" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="174" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="175"/>
-    </row>
-    <row r="4" spans="1:21" ht="13">
+      <c r="F3" s="156" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="157"/>
+    </row>
+    <row r="4" spans="1:22" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="178"/>
+      <c r="C4" s="153" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
-    </row>
-    <row r="5" spans="1:21" ht="13">
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
+    </row>
+    <row r="5" spans="1:22" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="178"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
-    </row>
-    <row r="6" spans="1:21" ht="13">
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
+    </row>
+    <row r="6" spans="1:22" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="153" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="178"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
-    </row>
-    <row r="7" spans="1:21" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
+    </row>
+    <row r="7" spans="1:22" ht="13">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
-    </row>
-    <row r="10" spans="1:21" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
-    </row>
-    <row r="12" spans="1:21" ht="12" thickBot="1">
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
+    </row>
+    <row r="10" spans="1:22" ht="12" thickBot="1">
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
+    </row>
+    <row r="12" spans="1:22" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -7496,7 +7658,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" s="30" t="s">
         <v>0</v>
       </c>
@@ -7528,37 +7690,40 @@
         <v>111</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O13" s="128" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P13" s="128" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="Q13" s="128" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="R13" s="128" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
       <c r="S13" s="128" t="s">
         <v>180</v>
       </c>
       <c r="T13" s="128" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="U13" s="128" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="17">
+        <v>225</v>
+      </c>
+      <c r="V13" s="128" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="17">
       <c r="A14" s="69">
         <v>1</v>
       </c>
@@ -7586,40 +7751,43 @@
         <v>108</v>
       </c>
       <c r="K14" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="M14" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="L14" s="13" t="s">
+      <c r="N14" s="136" t="s">
         <v>188</v>
-      </c>
-      <c r="M14" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="N14" s="136" t="s">
-        <v>190</v>
       </c>
       <c r="O14" s="13">
         <v>1</v>
       </c>
       <c r="P14" s="127" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q14" s="127" t="s">
         <v>191</v>
       </c>
-      <c r="Q14" s="127" t="s">
+      <c r="R14" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="R14" s="127" t="s">
+      <c r="S14" s="136" t="s">
         <v>193</v>
       </c>
-      <c r="S14" s="13" t="s">
+      <c r="T14" s="18" t="s">
         <v>194</v>
       </c>
-      <c r="T14" s="136" t="s">
-        <v>195</v>
-      </c>
-      <c r="U14" s="18" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" ht="17">
+      <c r="U14" s="127">
+        <v>41996.702777777777</v>
+      </c>
+      <c r="V14" s="127">
+        <v>41996.702777777777</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" ht="17">
       <c r="A15" s="59">
         <f>A14+1</f>
         <v>2</v>
@@ -7631,7 +7799,7 @@
         <v>105</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -7644,28 +7812,27 @@
       <c r="N15" s="136"/>
       <c r="P15" s="127"/>
       <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-    </row>
-    <row r="16" spans="1:21">
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A24" si="0">A15+1</f>
+        <f t="shared" ref="A16:A21" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C16" s="65" t="s">
         <v>111</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H16" s="87"/>
     </row>
@@ -7675,13 +7842,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
+        <v>159</v>
+      </c>
+      <c r="C17" s="65" t="s">
         <v>160</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="D17" s="65" t="s">
         <v>161</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>162</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
@@ -7696,13 +7863,13 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
+        <v>162</v>
+      </c>
+      <c r="C18" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="C18" s="65" t="s">
-        <v>164</v>
-      </c>
       <c r="D18" s="65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
@@ -7717,20 +7884,20 @@
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="65" t="s">
-        <v>166</v>
-      </c>
       <c r="D19" s="65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F19" s="67"/>
       <c r="G19" s="106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -7739,13 +7906,13 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="65" t="s">
         <v>168</v>
       </c>
-      <c r="C20" s="65" t="s">
-        <v>169</v>
-      </c>
       <c r="D20" s="129" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>3</v>
@@ -7754,7 +7921,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="106" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -7763,144 +7930,141 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="65" t="s">
         <v>170</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="D21" s="65" t="s">
         <v>171</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>172</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="59">
-        <f>A20+1</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="E22" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="67"/>
+      <c r="G22" s="106"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="139">
+        <v>10</v>
+      </c>
+      <c r="B23" s="140" t="s">
+        <v>177</v>
+      </c>
+      <c r="C23" s="141" t="s">
+        <v>178</v>
+      </c>
+      <c r="D23" s="65" t="s">
+        <v>161</v>
+      </c>
+      <c r="E23" s="142" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="143"/>
+      <c r="G23" s="144"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="139">
+        <v>11</v>
+      </c>
+      <c r="B24" s="140" t="s">
+        <v>179</v>
+      </c>
+      <c r="C24" s="141" t="s">
+        <v>180</v>
+      </c>
+      <c r="D24" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="E24" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="67"/>
-      <c r="G22" s="106" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="59">
-        <f>A21+1</f>
-        <v>9</v>
-      </c>
-      <c r="B23" s="63" t="s">
-        <v>212</v>
-      </c>
-      <c r="C23" s="65" t="s">
-        <v>213</v>
-      </c>
-      <c r="D23" s="65" t="s">
-        <v>148</v>
-      </c>
-      <c r="E23" s="66" t="s">
+      <c r="F24" s="143"/>
+      <c r="G24" s="144" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="59">
+        <v>12</v>
+      </c>
+      <c r="B25" s="202" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" s="203" t="s">
+        <v>184</v>
+      </c>
+      <c r="D25" s="203" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" s="204" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="205"/>
+      <c r="G25" s="206"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" s="69">
+        <v>13</v>
+      </c>
+      <c r="B26" s="197" t="s">
+        <v>205</v>
+      </c>
+      <c r="C26" s="198" t="s">
+        <v>206</v>
+      </c>
+      <c r="D26" s="198" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="199" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" s="59">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B24" s="63" t="s">
-        <v>176</v>
-      </c>
-      <c r="C24" s="65" t="s">
-        <v>177</v>
-      </c>
-      <c r="D24" s="65" t="s">
-        <v>178</v>
-      </c>
-      <c r="E24" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="67"/>
-      <c r="G24" s="106"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="139">
-        <v>11</v>
-      </c>
-      <c r="B25" s="140" t="s">
-        <v>179</v>
-      </c>
-      <c r="C25" s="141" t="s">
-        <v>180</v>
-      </c>
-      <c r="D25" s="65" t="s">
-        <v>162</v>
-      </c>
-      <c r="E25" s="142" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="143"/>
-      <c r="G25" s="144"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="139">
-        <v>12</v>
-      </c>
-      <c r="B26" s="140" t="s">
-        <v>181</v>
-      </c>
-      <c r="C26" s="141" t="s">
-        <v>182</v>
-      </c>
-      <c r="D26" s="65" t="s">
-        <v>183</v>
-      </c>
-      <c r="E26" s="142" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="143"/>
-      <c r="G26" s="144" t="s">
-        <v>184</v>
+      <c r="F26" s="200"/>
+      <c r="G26" s="201" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="12" thickBot="1">
       <c r="A27" s="70">
-        <v>13</v>
-      </c>
-      <c r="B27" s="131" t="s">
-        <v>185</v>
-      </c>
-      <c r="C27" s="132" t="s">
-        <v>186</v>
-      </c>
-      <c r="D27" s="132" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="133" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="135"/>
-      <c r="G27" s="134"/>
+        <v>14</v>
+      </c>
+      <c r="B27" s="207" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="68" t="s">
+        <v>208</v>
+      </c>
+      <c r="D27" s="68" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="208" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="209"/>
+      <c r="G27" s="210" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="29" spans="1:8" ht="12" thickBot="1">
       <c r="A29" s="1" t="s">
@@ -7935,10 +8099,10 @@
       <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="170" t="s">
+      <c r="C31" s="172" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="171"/>
+      <c r="D31" s="173"/>
       <c r="E31" s="46" t="s">
         <v>3</v>
       </c>
@@ -7952,8 +8116,8 @@
         <v>2</v>
       </c>
       <c r="B32" s="51"/>
-      <c r="C32" s="156"/>
-      <c r="D32" s="157"/>
+      <c r="C32" s="177"/>
+      <c r="D32" s="178"/>
       <c r="E32" s="52"/>
       <c r="F32" s="52"/>
       <c r="G32" s="53"/>
@@ -7963,8 +8127,8 @@
         <v>3</v>
       </c>
       <c r="B33" s="54"/>
-      <c r="C33" s="154"/>
-      <c r="D33" s="155"/>
+      <c r="C33" s="175"/>
+      <c r="D33" s="176"/>
       <c r="E33" s="58"/>
       <c r="F33" s="58"/>
       <c r="G33" s="55"/>
@@ -7981,14 +8145,14 @@
       <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="151" t="s">
+      <c r="C36" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D36" s="152"/>
-      <c r="E36" s="151" t="s">
+      <c r="D36" s="161"/>
+      <c r="E36" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F36" s="153"/>
+      <c r="F36" s="174"/>
       <c r="G36" s="38" t="s">
         <v>38</v>
       </c>
@@ -8005,45 +8169,45 @@
       <c r="B39" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="151" t="s">
+      <c r="C39" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="152"/>
-      <c r="E39" s="151" t="s">
+      <c r="D39" s="161"/>
+      <c r="E39" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="153"/>
+      <c r="F39" s="174"/>
       <c r="G39" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E36:F36"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="N14" r:id="rId1"/>
-    <hyperlink ref="T14" r:id="rId2"/>
+    <hyperlink ref="S14" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293"/>
@@ -8090,103 +8254,103 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="177"/>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="172" t="s">
+      <c r="F2" s="151" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="173"/>
+      <c r="G2" s="155"/>
     </row>
     <row r="3" spans="1:11" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="175"/>
+      <c r="G3" s="157"/>
     </row>
     <row r="4" spans="1:11" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
+      <c r="C4" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="178"/>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
     </row>
     <row r="5" spans="1:11" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="153" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="178"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
     </row>
     <row r="6" spans="1:11" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="153" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="178"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
     </row>
     <row r="7" spans="1:11" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:11" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:11" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8429,10 +8593,10 @@
       <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="170" t="s">
+      <c r="C25" s="172" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="171"/>
+      <c r="D25" s="173"/>
       <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
@@ -8468,14 +8632,14 @@
       <c r="B29" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="151" t="s">
+      <c r="C29" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="152"/>
-      <c r="E29" s="151" t="s">
+      <c r="D29" s="161"/>
+      <c r="E29" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F29" s="153"/>
+      <c r="F29" s="174"/>
       <c r="G29" s="38" t="s">
         <v>38</v>
       </c>
@@ -8492,14 +8656,14 @@
       <c r="B32" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="151" t="s">
+      <c r="C32" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="152"/>
-      <c r="E32" s="151" t="s">
+      <c r="D32" s="161"/>
+      <c r="E32" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="153"/>
+      <c r="F32" s="174"/>
       <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
@@ -8523,6 +8687,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8535,15 +8708,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8591,105 +8755,105 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="177"/>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="172" t="s">
+      <c r="F2" s="151" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="173"/>
+      <c r="G2" s="155"/>
     </row>
     <row r="3" spans="1:7" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="176" t="s">
+      <c r="F3" s="153" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="175"/>
+      <c r="G3" s="157"/>
     </row>
     <row r="4" spans="1:7" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
+      <c r="C4" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="178"/>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
     </row>
     <row r="5" spans="1:7" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="153" t="s">
         <v>89</v>
       </c>
-      <c r="D5" s="178"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
     </row>
     <row r="6" spans="1:7" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="153" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="178"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
     </row>
     <row r="7" spans="1:7" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="B8" s="163" t="s">
+      <c r="B8" s="165" t="s">
         <v>90</v>
       </c>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:7" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:7" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -8815,10 +8979,10 @@
       <c r="B20" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="170" t="s">
+      <c r="C20" s="172" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="171"/>
+      <c r="D20" s="173"/>
       <c r="E20" s="46" t="s">
         <v>3</v>
       </c>
@@ -8854,14 +9018,14 @@
       <c r="B24" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="151" t="s">
+      <c r="C24" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="152"/>
-      <c r="E24" s="151" t="s">
+      <c r="D24" s="161"/>
+      <c r="E24" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F24" s="153"/>
+      <c r="F24" s="174"/>
       <c r="G24" s="38" t="s">
         <v>38</v>
       </c>
@@ -8878,14 +9042,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="151" t="s">
+      <c r="C27" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="152"/>
-      <c r="E27" s="151" t="s">
+      <c r="D27" s="161"/>
+      <c r="E27" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F27" s="153"/>
+      <c r="F27" s="174"/>
       <c r="G27" s="38" t="s">
         <v>39</v>
       </c>
@@ -8903,6 +9067,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -8915,15 +9088,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8971,10 +9135,10 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
+      <c r="C2" s="151" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="177"/>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
@@ -8987,87 +9151,87 @@
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="174" t="s">
+      <c r="F3" s="156" t="s">
         <v>99</v>
       </c>
-      <c r="G3" s="175"/>
+      <c r="G3" s="157"/>
     </row>
     <row r="4" spans="1:14" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
+      <c r="C4" s="153" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="178"/>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
     </row>
     <row r="5" spans="1:14" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="153" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="178"/>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
     </row>
     <row r="6" spans="1:14" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
+      <c r="C6" s="153" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="178"/>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
     </row>
     <row r="7" spans="1:14" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:14">
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:14">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:14" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="11" spans="1:14">
       <c r="H11" s="87"/>
@@ -9310,10 +9474,10 @@
       <c r="B22" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="170" t="s">
+      <c r="C22" s="172" t="s">
         <v>57</v>
       </c>
-      <c r="D22" s="171"/>
+      <c r="D22" s="173"/>
       <c r="E22" s="46" t="s">
         <v>3</v>
       </c>
@@ -9333,10 +9497,10 @@
         <v>2</v>
       </c>
       <c r="B23" s="51"/>
-      <c r="C23" s="156" t="s">
+      <c r="C23" s="177" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="157"/>
+      <c r="D23" s="178"/>
       <c r="E23" s="52"/>
       <c r="F23" s="52" t="s">
         <v>3</v>
@@ -9396,14 +9560,14 @@
       <c r="B27" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C27" s="151" t="s">
+      <c r="C27" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="152"/>
-      <c r="E27" s="151" t="s">
+      <c r="D27" s="161"/>
+      <c r="E27" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="153"/>
+      <c r="F27" s="174"/>
       <c r="G27" s="38" t="s">
         <v>38</v>
       </c>
@@ -9440,14 +9604,14 @@
       <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="151" t="s">
+      <c r="C30" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D30" s="152"/>
-      <c r="E30" s="151" t="s">
+      <c r="D30" s="161"/>
+      <c r="E30" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="153"/>
+      <c r="F30" s="174"/>
       <c r="G30" s="38" t="s">
         <v>39</v>
       </c>
@@ -9463,14 +9627,14 @@
         <v>1</v>
       </c>
       <c r="B31" s="51"/>
-      <c r="C31" s="170" t="s">
+      <c r="C31" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="D31" s="171"/>
-      <c r="E31" s="156" t="s">
+      <c r="D31" s="173"/>
+      <c r="E31" s="177" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="157"/>
+      <c r="F31" s="178"/>
       <c r="G31" s="53" t="s">
         <v>76</v>
       </c>
@@ -9546,14 +9710,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B7:G7"/>
-    <mergeCell ref="B8:G10"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="C31:D31"/>
@@ -9570,6 +9726,14 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B7:G7"/>
+    <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C23:D23"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9591,10 +9755,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="K3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
@@ -9624,101 +9788,101 @@
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="177"/>
+      <c r="C2" s="151" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="172"/>
-      <c r="G2" s="173"/>
+      <c r="F2" s="151"/>
+      <c r="G2" s="155"/>
     </row>
     <row r="3" spans="1:19" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="174" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="175"/>
+      <c r="F3" s="156" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="157"/>
     </row>
     <row r="4" spans="1:19" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="178"/>
+      <c r="C4" s="153" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
     </row>
     <row r="5" spans="1:19" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
-        <v>217</v>
-      </c>
-      <c r="D5" s="178"/>
+      <c r="C5" s="153" t="s">
+        <v>212</v>
+      </c>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
     </row>
     <row r="6" spans="1:19" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
-        <v>218</v>
-      </c>
-      <c r="D6" s="178"/>
+      <c r="C6" s="153" t="s">
+        <v>213</v>
+      </c>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
     </row>
     <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
     </row>
     <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
     </row>
     <row r="12" spans="1:19" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
@@ -9754,25 +9918,29 @@
         <v>109</v>
       </c>
       <c r="J13" s="128" t="s">
+        <v>142</v>
+      </c>
+      <c r="K13" s="128" t="s">
         <v>143</v>
       </c>
-      <c r="K13" s="128" t="s">
-        <v>144</v>
-      </c>
       <c r="L13" s="128" t="s">
-        <v>114</v>
+        <v>227</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>114</v>
+        <v>229</v>
       </c>
       <c r="O13" s="128" t="s">
-        <v>114</v>
-      </c>
-      <c r="P13" s="128"/>
-      <c r="Q13" s="128"/>
+        <v>230</v>
+      </c>
+      <c r="P13" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q13" s="128" t="s">
+        <v>226</v>
+      </c>
       <c r="R13" s="128"/>
       <c r="S13" s="128"/>
     </row>
@@ -9801,14 +9969,29 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K14" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="N14" s="136"/>
-      <c r="P14" s="127"/>
-      <c r="Q14" s="127"/>
+        <v>146</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="N14" s="136">
+        <v>1</v>
+      </c>
+      <c r="O14" s="13">
+        <v>1</v>
+      </c>
+      <c r="P14" s="127">
+        <v>41996.620833333334</v>
+      </c>
+      <c r="Q14" s="127">
+        <v>41996.620833333334</v>
+      </c>
       <c r="R14" s="127"/>
     </row>
     <row r="15" spans="1:19" ht="17">
@@ -9817,13 +10000,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -9835,32 +10018,47 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="K15" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="N15" s="136"/>
-      <c r="P15" s="127"/>
-      <c r="Q15" s="127"/>
+      <c r="L15" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="N15" s="136">
+        <v>1</v>
+      </c>
+      <c r="O15" s="13">
+        <v>1</v>
+      </c>
+      <c r="P15" s="127">
+        <v>41996.620833333334</v>
+      </c>
+      <c r="Q15" s="127">
+        <v>41996.620833333334</v>
+      </c>
       <c r="R15" s="127"/>
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A24" si="0">A15+1</f>
+        <f t="shared" ref="A16:A23" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C16" s="65" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="65" t="s">
         <v>123</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="E16" s="66" t="s">
         <v>124</v>
-      </c>
-      <c r="E16" s="66" t="s">
-        <v>125</v>
       </c>
       <c r="F16" s="67"/>
       <c r="G16" s="117"/>
@@ -9872,16 +10070,16 @@
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C17" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D17" s="65" t="s">
         <v>127</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="E17" s="66" t="s">
         <v>128</v>
-      </c>
-      <c r="E17" s="66" t="s">
-        <v>129</v>
       </c>
       <c r="F17" s="67"/>
       <c r="G17" s="117"/>
@@ -9892,43 +10090,38 @@
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="C18" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="129" t="s">
         <v>130</v>
       </c>
-      <c r="D18" s="129" t="s">
-        <v>131</v>
-      </c>
       <c r="E18" s="66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F18" s="67"/>
       <c r="G18" s="106"/>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="59">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="129" t="s">
-        <v>208</v>
+        <v>140</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>141</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="146" t="s">
-        <v>134</v>
-      </c>
-      <c r="G19" s="106" t="s">
-        <v>207</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F19" s="67"/>
+      <c r="G19" s="106"/>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" s="59">
@@ -9936,20 +10129,22 @@
         <v>7</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>214</v>
+        <v>131</v>
       </c>
       <c r="C20" s="65" t="s">
-        <v>215</v>
+        <v>132</v>
       </c>
       <c r="D20" s="129" t="s">
-        <v>149</v>
+        <v>203</v>
       </c>
       <c r="E20" s="66" t="s">
-        <v>125</v>
-      </c>
-      <c r="F20" s="67"/>
+        <v>124</v>
+      </c>
+      <c r="F20" s="146" t="s">
+        <v>133</v>
+      </c>
       <c r="G20" s="106" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -9958,20 +10153,20 @@
         <v>8</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c r="C21" s="65" t="s">
-        <v>216</v>
-      </c>
-      <c r="D21" s="65" t="s">
-        <v>150</v>
+        <v>210</v>
+      </c>
+      <c r="D21" s="129" t="s">
+        <v>148</v>
       </c>
       <c r="E21" s="66" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="F21" s="67"/>
       <c r="G21" s="106" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -9980,188 +10175,168 @@
         <v>9</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C22" s="65" t="s">
-        <v>141</v>
+        <v>211</v>
       </c>
       <c r="D22" s="65" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="E22" s="66" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F22" s="67"/>
-      <c r="G22" s="106"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="59">
+      <c r="G22" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="12" thickBot="1">
+      <c r="A23" s="70">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B23" s="63"/>
-      <c r="C23" s="65"/>
-      <c r="D23" s="65"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="106"/>
-    </row>
-    <row r="24" spans="1:7" ht="12" thickBot="1">
-      <c r="A24" s="70">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B24" s="131"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="135"/>
-      <c r="G24" s="134"/>
-    </row>
-    <row r="26" spans="1:7" ht="12" thickBot="1">
-      <c r="A26" s="1" t="s">
+      <c r="B23" s="131"/>
+      <c r="C23" s="132"/>
+      <c r="D23" s="132"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="135"/>
+      <c r="G23" s="134"/>
+    </row>
+    <row r="25" spans="1:7" ht="12" thickBot="1">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="29" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="158" t="s">
+      <c r="C26" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D27" s="159"/>
-      <c r="E27" s="34" t="s">
+      <c r="D26" s="159"/>
+      <c r="E26" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="F26" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G27" s="35" t="s">
+      <c r="G26" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13">
-      <c r="A28" s="14">
+    <row r="27" spans="1:7" ht="13">
+      <c r="A27" s="14">
         <v>1</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B27" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="170" t="s">
+      <c r="C27" s="172" t="s">
         <v>109</v>
       </c>
-      <c r="D28" s="171"/>
-      <c r="E28" s="46" t="s">
+      <c r="D27" s="173"/>
+      <c r="E27" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="46" t="s">
+      <c r="F27" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="13" customHeight="1">
-      <c r="A29" s="57">
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="1:7" ht="13" customHeight="1">
+      <c r="A28" s="57">
         <v>2</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="156"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="52"/>
-      <c r="G29" s="53"/>
-    </row>
-    <row r="30" spans="1:7" ht="13" customHeight="1" thickBot="1">
-      <c r="A30" s="56">
+      <c r="B28" s="51"/>
+      <c r="C28" s="177"/>
+      <c r="D28" s="178"/>
+      <c r="E28" s="52"/>
+      <c r="F28" s="52"/>
+      <c r="G28" s="53"/>
+    </row>
+    <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
+      <c r="A29" s="56">
         <v>3</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="154"/>
-      <c r="D30" s="155"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="55"/>
-    </row>
-    <row r="32" spans="1:7" ht="12" thickBot="1">
-      <c r="A32" s="1" t="s">
+      <c r="B29" s="54"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="176"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="55"/>
+    </row>
+    <row r="31" spans="1:7" ht="12" thickBot="1">
+      <c r="A31" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="14" thickBot="1">
+      <c r="A32" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="161"/>
+      <c r="E32" s="160" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="174"/>
+      <c r="G32" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="13">
+      <c r="A33" s="14">
+        <v>1</v>
+      </c>
+      <c r="B33" s="19"/>
+      <c r="C33" s="172" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="173"/>
+      <c r="E33" s="187" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="14" thickBot="1">
-      <c r="A33" s="36" t="s">
+      <c r="F33" s="188"/>
+      <c r="G33" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="12" thickBot="1">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="14" thickBot="1">
+      <c r="A36" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="151" t="s">
+      <c r="C36" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D33" s="152"/>
-      <c r="E33" s="151" t="s">
-        <v>36</v>
-      </c>
-      <c r="F33" s="153"/>
-      <c r="G33" s="38" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="13">
-      <c r="A34" s="14">
-        <v>1</v>
-      </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="170" t="s">
-        <v>138</v>
-      </c>
-      <c r="D34" s="171"/>
-      <c r="E34" s="187" t="s">
-        <v>152</v>
-      </c>
-      <c r="F34" s="188"/>
-      <c r="G34" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="12" thickBot="1">
-      <c r="A36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="14" thickBot="1">
-      <c r="A37" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="C37" s="151" t="s">
-        <v>44</v>
-      </c>
-      <c r="D37" s="152"/>
-      <c r="E37" s="151" t="s">
+      <c r="D36" s="161"/>
+      <c r="E36" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F37" s="153"/>
-      <c r="G37" s="38" t="s">
+      <c r="F36" s="174"/>
+      <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="E33:F33"/>
     <mergeCell ref="B8:G10"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="F2:G2"/>
@@ -10174,6 +10349,16 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F32"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10195,9 +10380,11 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S38"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11" x14ac:dyDescent="0"/>
   <cols>
@@ -10210,119 +10397,118 @@
     <col min="9" max="10" width="8.83203125" style="13"/>
     <col min="11" max="11" width="17.6640625" style="13" customWidth="1"/>
     <col min="12" max="12" width="12.6640625" style="13" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="13" customWidth="1"/>
-    <col min="14" max="15" width="19.33203125" style="13" customWidth="1"/>
-    <col min="16" max="17" width="17" style="13" customWidth="1"/>
-    <col min="18" max="18" width="15.5" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="8.83203125" style="13"/>
+    <col min="13" max="14" width="19.33203125" style="13" customWidth="1"/>
+    <col min="15" max="16" width="17" style="13" customWidth="1"/>
+    <col min="17" max="17" width="15.5" style="13" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="12" thickBot="1">
+    <row r="1" spans="1:18" ht="12" thickBot="1">
       <c r="A1" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" ht="13">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="13">
       <c r="B2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="172" t="s">
-        <v>115</v>
-      </c>
-      <c r="D2" s="177"/>
+      <c r="C2" s="151" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" s="152"/>
       <c r="E2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="172"/>
-      <c r="G2" s="173"/>
-    </row>
-    <row r="3" spans="1:19" ht="13">
+      <c r="F2" s="151"/>
+      <c r="G2" s="155"/>
+    </row>
+    <row r="3" spans="1:18" ht="13">
       <c r="B3" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="176"/>
-      <c r="D3" s="178"/>
+      <c r="C3" s="153"/>
+      <c r="D3" s="154"/>
       <c r="E3" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="174" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="175"/>
-    </row>
-    <row r="4" spans="1:19" ht="13">
+      <c r="F3" s="156" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="157"/>
+    </row>
+    <row r="4" spans="1:18" ht="13">
       <c r="B4" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="176" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="178"/>
+      <c r="C4" s="153" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="154"/>
       <c r="E4" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="176"/>
-      <c r="G4" s="175"/>
-    </row>
-    <row r="5" spans="1:19" ht="13">
+      <c r="F4" s="153"/>
+      <c r="G4" s="157"/>
+    </row>
+    <row r="5" spans="1:18" ht="13">
       <c r="B5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="176" t="s">
-        <v>227</v>
-      </c>
-      <c r="D5" s="178"/>
+      <c r="C5" s="153" t="s">
+        <v>222</v>
+      </c>
+      <c r="D5" s="154"/>
       <c r="E5" s="42"/>
-      <c r="F5" s="176"/>
-      <c r="G5" s="175"/>
-    </row>
-    <row r="6" spans="1:19" ht="13">
+      <c r="F5" s="153"/>
+      <c r="G5" s="157"/>
+    </row>
+    <row r="6" spans="1:18" ht="13">
       <c r="B6" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="176" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" s="178"/>
+      <c r="C6" s="153" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="154"/>
       <c r="E6" s="43"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="175"/>
-    </row>
-    <row r="7" spans="1:19" ht="13">
-      <c r="B7" s="160" t="s">
+      <c r="F6" s="153"/>
+      <c r="G6" s="157"/>
+    </row>
+    <row r="7" spans="1:18" ht="13">
+      <c r="B7" s="162" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="161"/>
-      <c r="D7" s="161"/>
-      <c r="E7" s="161"/>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="B8" s="163"/>
-      <c r="C8" s="164"/>
-      <c r="D8" s="164"/>
-      <c r="E8" s="164"/>
-      <c r="F8" s="164"/>
-      <c r="G8" s="165"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="B9" s="166"/>
-      <c r="C9" s="164"/>
-      <c r="D9" s="164"/>
-      <c r="E9" s="164"/>
-      <c r="F9" s="164"/>
-      <c r="G9" s="165"/>
-    </row>
-    <row r="10" spans="1:19" ht="12" thickBot="1">
-      <c r="B10" s="167"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="168"/>
-      <c r="E10" s="168"/>
-      <c r="F10" s="168"/>
-      <c r="G10" s="169"/>
-    </row>
-    <row r="12" spans="1:19" ht="12" thickBot="1">
+      <c r="C7" s="163"/>
+      <c r="D7" s="163"/>
+      <c r="E7" s="163"/>
+      <c r="F7" s="163"/>
+      <c r="G7" s="164"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="166"/>
+      <c r="E8" s="166"/>
+      <c r="F8" s="166"/>
+      <c r="G8" s="167"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="B9" s="168"/>
+      <c r="C9" s="166"/>
+      <c r="D9" s="166"/>
+      <c r="E9" s="166"/>
+      <c r="F9" s="166"/>
+      <c r="G9" s="167"/>
+    </row>
+    <row r="10" spans="1:18" ht="12" thickBot="1">
+      <c r="B10" s="169"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="171"/>
+    </row>
+    <row r="12" spans="1:18" ht="12" thickBot="1">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -10330,7 +10516,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:18">
       <c r="A13" s="30" t="s">
         <v>0</v>
       </c>
@@ -10356,29 +10542,26 @@
         <v>109</v>
       </c>
       <c r="J13" s="128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K13" s="128" t="s">
-        <v>200</v>
+        <v>233</v>
       </c>
       <c r="L13" s="128" t="s">
-        <v>202</v>
+        <v>234</v>
       </c>
       <c r="M13" s="128" t="s">
-        <v>6</v>
+        <v>235</v>
       </c>
       <c r="N13" s="128" t="s">
-        <v>137</v>
-      </c>
-      <c r="O13" s="128" t="s">
-        <v>204</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="O13" s="128"/>
       <c r="P13" s="128"/>
       <c r="Q13" s="128"/>
       <c r="R13" s="128"/>
-      <c r="S13" s="128"/>
-    </row>
-    <row r="14" spans="1:19">
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="69">
         <v>1</v>
       </c>
@@ -10403,28 +10586,25 @@
         <v>1</v>
       </c>
       <c r="J14" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="K14" s="127" t="s">
-        <v>192</v>
-      </c>
-      <c r="L14" s="127" t="s">
-        <v>192</v>
-      </c>
-      <c r="M14" s="13">
+        <v>200</v>
+      </c>
+      <c r="K14" s="211">
         <v>1</v>
       </c>
-      <c r="N14" s="13">
-        <v>2</v>
-      </c>
-      <c r="O14" s="13">
+      <c r="L14" s="211">
         <v>1</v>
       </c>
+      <c r="M14" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="N14" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="O14" s="127"/>
       <c r="P14" s="127"/>
       <c r="Q14" s="127"/>
-      <c r="R14" s="127"/>
-    </row>
-    <row r="15" spans="1:19">
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="59">
         <f>A14+1</f>
         <v>2</v>
@@ -10433,10 +10613,10 @@
         <v>12</v>
       </c>
       <c r="C15" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D15" s="65" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>3</v>
@@ -10448,113 +10628,110 @@
         <v>2</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="K15" s="127" t="s">
-        <v>192</v>
-      </c>
-      <c r="L15" s="127" t="s">
-        <v>192</v>
-      </c>
-      <c r="M15" s="13">
-        <v>0</v>
-      </c>
-      <c r="N15" s="13">
+        <v>201</v>
+      </c>
+      <c r="K15" s="211">
         <v>1</v>
       </c>
-      <c r="O15" s="13">
+      <c r="L15" s="211">
         <v>2</v>
       </c>
+      <c r="M15" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="N15" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="O15" s="127"/>
       <c r="P15" s="127"/>
       <c r="Q15" s="127"/>
-      <c r="R15" s="127"/>
-    </row>
-    <row r="16" spans="1:19">
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="59">
-        <f t="shared" ref="A16:A17" si="0">A15+1</f>
         <v>3</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>199</v>
+        <v>138</v>
       </c>
       <c r="C16" s="65" t="s">
-        <v>200</v>
+        <v>136</v>
       </c>
       <c r="D16" s="65" t="s">
-        <v>148</v>
+        <v>53</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F16" s="67"/>
-      <c r="G16" s="106" t="s">
-        <v>175</v>
-      </c>
-      <c r="H16" s="87"/>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="G16" s="106"/>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" s="59">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="C17" s="65" t="s">
-        <v>202</v>
-      </c>
-      <c r="D17" s="65" t="s">
-        <v>148</v>
+        <v>215</v>
+      </c>
+      <c r="D17" s="129" t="s">
+        <v>53</v>
       </c>
       <c r="E17" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F17" s="67"/>
-      <c r="G17" s="106" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="F17" s="138"/>
+      <c r="G17" s="106"/>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" s="59">
+        <f t="shared" ref="A18:A19" si="0">A17+1</f>
         <v>5</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>139</v>
+        <v>197</v>
       </c>
       <c r="C18" s="65" t="s">
-        <v>137</v>
+        <v>223</v>
       </c>
       <c r="D18" s="65" t="s">
-        <v>53</v>
+        <v>147</v>
       </c>
       <c r="E18" s="66" t="s">
         <v>3</v>
       </c>
       <c r="F18" s="67"/>
-      <c r="G18" s="106"/>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="G18" s="106" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" s="87"/>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="59">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C19" s="65" t="s">
-        <v>220</v>
-      </c>
-      <c r="D19" s="129" t="s">
-        <v>53</v>
+        <v>224</v>
+      </c>
+      <c r="D19" s="65" t="s">
+        <v>147</v>
       </c>
       <c r="E19" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F19" s="138"/>
-      <c r="G19" s="106"/>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="F19" s="67"/>
+      <c r="G19" s="106" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" s="59">
-        <f t="shared" ref="A20:A23" si="1">A19+1</f>
+        <f t="shared" ref="A20:A21" si="1">A19+1</f>
         <v>7</v>
       </c>
       <c r="B20" s="63"/>
@@ -10564,230 +10741,206 @@
       <c r="F20" s="67"/>
       <c r="G20" s="106"/>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="59">
+    <row r="21" spans="1:8" ht="12" thickBot="1">
+      <c r="A21" s="70">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="106"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="59">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="B22" s="63"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="106"/>
-    </row>
-    <row r="23" spans="1:7" ht="12" thickBot="1">
-      <c r="A23" s="70">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B23" s="131"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="135"/>
-      <c r="G23" s="134"/>
-    </row>
-    <row r="25" spans="1:7" ht="12" thickBot="1">
-      <c r="A25" s="1" t="s">
+      <c r="B21" s="131"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="132"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="135"/>
+      <c r="G21" s="134"/>
+    </row>
+    <row r="23" spans="1:8" ht="12" thickBot="1">
+      <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="29" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B24" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="158" t="s">
+      <c r="C24" s="158" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="159"/>
-      <c r="E26" s="34" t="s">
+      <c r="D24" s="159"/>
+      <c r="E24" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="34" t="s">
+      <c r="F24" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="35" t="s">
+      <c r="G24" s="35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13">
-      <c r="A27" s="14">
+    <row r="25" spans="1:8" ht="13">
+      <c r="A25" s="14">
         <v>1</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B25" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="170" t="s">
+      <c r="C25" s="172" t="s">
         <v>109</v>
       </c>
-      <c r="D27" s="171"/>
-      <c r="E27" s="46" t="s">
+      <c r="D25" s="173"/>
+      <c r="E25" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F27" s="46" t="s">
+      <c r="F25" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:7" ht="13" customHeight="1">
-      <c r="A28" s="57">
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" ht="13" customHeight="1">
+      <c r="A26" s="57">
         <v>2</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="46"/>
-      <c r="F28" s="46"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" ht="13" customHeight="1" thickBot="1">
-      <c r="A29" s="56">
+      <c r="B26" s="51"/>
+      <c r="C26" s="177"/>
+      <c r="D26" s="178"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" ht="13" customHeight="1" thickBot="1">
+      <c r="A27" s="56">
         <v>3</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="154"/>
-      <c r="D29" s="155"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="55"/>
-    </row>
-    <row r="31" spans="1:7" ht="12" thickBot="1">
-      <c r="A31" s="1" t="s">
+      <c r="B27" s="54"/>
+      <c r="C27" s="175"/>
+      <c r="D27" s="176"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="55"/>
+    </row>
+    <row r="29" spans="1:8" ht="12" thickBot="1">
+      <c r="A29" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="14" thickBot="1">
-      <c r="A32" s="36" t="s">
+    <row r="30" spans="1:8" ht="14" thickBot="1">
+      <c r="A30" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B30" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C32" s="151" t="s">
+      <c r="C30" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D32" s="152"/>
-      <c r="E32" s="151" t="s">
+      <c r="D30" s="161"/>
+      <c r="E30" s="160" t="s">
         <v>36</v>
       </c>
-      <c r="F32" s="153"/>
-      <c r="G32" s="38" t="s">
+      <c r="F30" s="174"/>
+      <c r="G30" s="38" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="14">
+    <row r="31" spans="1:8">
+      <c r="A31" s="14">
         <v>1</v>
       </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="187" t="s">
-        <v>221</v>
-      </c>
-      <c r="D33" s="188"/>
-      <c r="E33" s="191" t="s">
-        <v>203</v>
-      </c>
-      <c r="F33" s="192"/>
-      <c r="G33" s="20" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="14">
+      <c r="B31" s="19"/>
+      <c r="C31" s="187" t="s">
+        <v>216</v>
+      </c>
+      <c r="D31" s="188"/>
+      <c r="E31" s="191" t="s">
+        <v>199</v>
+      </c>
+      <c r="F31" s="192"/>
+      <c r="G31" s="20" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="14">
         <v>1</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="189" t="s">
-        <v>223</v>
-      </c>
-      <c r="D34" s="190"/>
-      <c r="E34" s="193" t="s">
+      <c r="B32" s="19"/>
+      <c r="C32" s="189" t="s">
         <v>218</v>
       </c>
-      <c r="F34" s="194"/>
-      <c r="G34" s="20" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="14" customHeight="1" thickBot="1">
-      <c r="A35" s="56">
+      <c r="D32" s="190"/>
+      <c r="E32" s="193" t="s">
+        <v>213</v>
+      </c>
+      <c r="F32" s="194"/>
+      <c r="G32" s="20" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="14" customHeight="1" thickBot="1">
+      <c r="A33" s="56">
         <v>3</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="154"/>
-      <c r="D35" s="155"/>
-      <c r="E35" s="195"/>
-      <c r="F35" s="196"/>
-      <c r="G35" s="55"/>
-    </row>
-    <row r="37" spans="1:7" ht="12" thickBot="1">
-      <c r="A37" s="1" t="s">
+      <c r="B33" s="54"/>
+      <c r="C33" s="175"/>
+      <c r="D33" s="176"/>
+      <c r="E33" s="195"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="55"/>
+    </row>
+    <row r="35" spans="1:7" ht="12" thickBot="1">
+      <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="12" thickBot="1">
-      <c r="A38" s="36" t="s">
+    <row r="36" spans="1:7" ht="12" thickBot="1">
+      <c r="A36" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B36" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="151" t="s">
+      <c r="C36" s="160" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="152"/>
-      <c r="E38" s="151" t="s">
+      <c r="D36" s="161"/>
+      <c r="E36" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="152"/>
-      <c r="G38" s="38" t="s">
+      <c r="F36" s="161"/>
+      <c r="G36" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G10"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>